<commit_message>
Completed Control Decode. Fixed Error with ALU Op and Opcode conflict dealing with BRANCH class instructions.
</commit_message>
<xml_diff>
--- a/materials/Instructions.xlsx
+++ b/materials/Instructions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingi\Documents\UTD\4310 Arch\Project\materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4827AA3-42FF-440B-88B9-95D03595E6A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BC1AB9-F7EE-48A5-82B3-2C294E1BC3E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction Types" sheetId="1" r:id="rId1"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="245">
   <si>
     <t>Opcode</t>
   </si>
@@ -429,9 +429,6 @@
     <t>Select pc</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>Select 4</t>
   </si>
   <si>
@@ -832,6 +829,12 @@
   </si>
   <si>
     <t>Opcodes</t>
+  </si>
+  <si>
+    <t>kk</t>
+  </si>
+  <si>
+    <t>SE imm_big</t>
   </si>
 </sst>
 </file>
@@ -1059,6 +1062,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1074,10 +1081,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1367,7 +1370,7 @@
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="J10" sqref="J10:U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
@@ -1379,38 +1382,38 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25" t="s">
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25" t="s">
+      <c r="I1" s="29"/>
+      <c r="J1" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25" t="s">
+      <c r="K1" s="29"/>
+      <c r="L1" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="25"/>
-      <c r="N1" s="26" t="s">
+      <c r="M1" s="29"/>
+      <c r="N1" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="28"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="32"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
@@ -1419,36 +1422,36 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25" t="s">
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25" t="s">
+      <c r="I3" s="29"/>
+      <c r="J3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="25"/>
-      <c r="L3" s="26" t="s">
+      <c r="K3" s="29"/>
+      <c r="L3" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="27"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="U3" s="28"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="32"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
@@ -1459,34 +1462,34 @@
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="26" t="s">
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="28"/>
-      <c r="J5" s="26" t="s">
+      <c r="I5" s="32"/>
+      <c r="J5" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="28"/>
-      <c r="L5" s="26" t="s">
+      <c r="K5" s="32"/>
+      <c r="L5" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="27"/>
-      <c r="S5" s="27"/>
-      <c r="T5" s="27"/>
-      <c r="U5" s="28"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="32"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
@@ -1495,41 +1498,41 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A8" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B8" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="26" t="s">
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="28"/>
-      <c r="J8" s="26" t="s">
+      <c r="I8" s="32"/>
+      <c r="J8" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="28"/>
-      <c r="L8" s="26" t="s">
+      <c r="K8" s="32"/>
+      <c r="L8" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="27"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="27"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="27"/>
-      <c r="R8" s="27"/>
-      <c r="S8" s="27"/>
-      <c r="T8" s="27"/>
-      <c r="U8" s="28"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="31"/>
+      <c r="T8" s="31"/>
+      <c r="U8" s="32"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
@@ -1543,34 +1546,34 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A11" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B11" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="26" t="s">
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="I11" s="28"/>
-      <c r="J11" s="26" t="s">
+      <c r="I11" s="32"/>
+      <c r="J11" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="27"/>
-      <c r="S11" s="27"/>
-      <c r="T11" s="27"/>
-      <c r="U11" s="28"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="31"/>
+      <c r="T11" s="31"/>
+      <c r="U11" s="32"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
@@ -1581,32 +1584,32 @@
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="26" t="s">
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="26" t="s">
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="32"/>
+      <c r="Q13" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="R13" s="27"/>
-      <c r="S13" s="27"/>
-      <c r="T13" s="27"/>
-      <c r="U13" s="28"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="31"/>
+      <c r="T13" s="31"/>
+      <c r="U13" s="32"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
@@ -1615,14 +1618,11 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:U3"/>
-    <mergeCell ref="L5:U5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:U1"/>
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="B8:G8"/>
     <mergeCell ref="H8:I8"/>
@@ -1633,11 +1633,14 @@
     <mergeCell ref="J11:U11"/>
     <mergeCell ref="Q13:U13"/>
     <mergeCell ref="H13:P13"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:U3"/>
+    <mergeCell ref="L5:U5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1648,8 +1651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2897DEC3-240E-431E-8285-E03640E230E7}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.5" x14ac:dyDescent="0.45"/>
@@ -1669,50 +1672,50 @@
         <v>38</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>121</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>122</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>45</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
+      <c r="B2" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
     </row>
     <row r="3" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
+      <c r="B3" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
       <c r="G3" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="57" x14ac:dyDescent="0.45">
@@ -1723,16 +1726,16 @@
         <v>50</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>53</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G4" s="18"/>
     </row>
@@ -1741,7 +1744,7 @@
         <v>42</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C5" s="35"/>
       <c r="D5" s="6"/>
@@ -1759,7 +1762,7 @@
       <c r="C6" s="18"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
@@ -1780,7 +1783,7 @@
     </row>
     <row r="10" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
@@ -1856,23 +1859,23 @@
       <c r="A47" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B47" s="29" t="s">
+      <c r="B47" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="33"/>
+      <c r="E47" s="33"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B48" s="29" t="s">
+      <c r="B48" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="C48" s="29"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="29"/>
+      <c r="C48" s="33"/>
+      <c r="D48" s="33"/>
+      <c r="E48" s="33"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" s="5" t="s">
@@ -1933,23 +1936,23 @@
       <c r="A54" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B54" s="29" t="s">
+      <c r="B54" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="C54" s="29"/>
-      <c r="D54" s="29"/>
-      <c r="E54" s="29"/>
+      <c r="C54" s="33"/>
+      <c r="D54" s="33"/>
+      <c r="E54" s="33"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B55" s="29" t="s">
+      <c r="B55" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C55" s="29"/>
-      <c r="D55" s="29"/>
-      <c r="E55" s="29"/>
+      <c r="C55" s="33"/>
+      <c r="D55" s="33"/>
+      <c r="E55" s="33"/>
     </row>
     <row r="56" spans="1:5" ht="57" x14ac:dyDescent="0.45">
       <c r="A56" s="5" t="s">
@@ -2040,8 +2043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E23297D-859B-4DF0-AD52-FCC5F95569EC}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
@@ -2061,374 +2064,374 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.5">
       <c r="B1" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>218</v>
-      </c>
-      <c r="F1" s="32"/>
+        <v>175</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="F1" s="27"/>
       <c r="G1" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H1" s="15"/>
-      <c r="I1" s="32"/>
+      <c r="I1" s="27"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A2" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="B2" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="H2" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="E2" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>207</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="H2" s="33" t="s">
-        <v>178</v>
-      </c>
-      <c r="I2" s="32"/>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A3" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>204</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>184</v>
-      </c>
-      <c r="F3" s="33" t="s">
-        <v>208</v>
-      </c>
-      <c r="G3" s="33" t="s">
-        <v>195</v>
-      </c>
-      <c r="H3" s="33" t="s">
-        <v>179</v>
-      </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="30"/>
+        <v>120</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="I3" s="27"/>
+      <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A4" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>182</v>
-      </c>
-      <c r="E4" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>209</v>
-      </c>
-      <c r="G4" s="33" t="s">
-        <v>196</v>
-      </c>
-      <c r="H4" s="33" t="s">
-        <v>180</v>
-      </c>
-      <c r="I4" s="33"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
+        <v>121</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>208</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="I4" s="28"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A5" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="30" t="s">
-        <v>183</v>
-      </c>
-      <c r="E5" s="33" t="s">
-        <v>186</v>
-      </c>
-      <c r="F5" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="G5" s="33" t="s">
-        <v>197</v>
-      </c>
-      <c r="H5" s="33" t="s">
-        <v>181</v>
-      </c>
-      <c r="I5" s="33"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
+      <c r="B5" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="I5" s="28"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A6" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>205</v>
-      </c>
-      <c r="E6" s="33" t="s">
-        <v>187</v>
-      </c>
-      <c r="F6" s="33" t="s">
-        <v>211</v>
-      </c>
-      <c r="G6" s="33" t="s">
-        <v>198</v>
-      </c>
-      <c r="H6" s="33" t="s">
-        <v>182</v>
-      </c>
-      <c r="I6" s="33"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
+        <v>122</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>210</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="I6" s="28"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A7" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="E7" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="I7" s="28"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="E8" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="F8" s="28" t="s">
         <v>212</v>
-      </c>
-      <c r="G7" s="33" t="s">
-        <v>199</v>
-      </c>
-      <c r="H7" s="33" t="s">
-        <v>183</v>
-      </c>
-      <c r="I7" s="33"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="E8" s="33" t="s">
-        <v>189</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>213</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="I9" s="28"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="E10" s="28" t="s">
         <v>190</v>
       </c>
-      <c r="F9" s="33" t="s">
+      <c r="F10" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G9" s="33" t="s">
+      <c r="G10" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="H9" s="33" t="s">
-        <v>178</v>
-      </c>
-      <c r="I9" s="33"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="E10" s="33" t="s">
+      <c r="H10" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="I10" s="28"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="E11" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="F10" s="33" t="s">
+      <c r="F11" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G10" s="33" t="s">
+      <c r="G11" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="E12" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="G12" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="H10" s="33" t="s">
-        <v>182</v>
-      </c>
-      <c r="I10" s="33"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="E11" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="F11" s="33" t="s">
-        <v>216</v>
-      </c>
-      <c r="G11" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="E12" s="33" t="s">
-        <v>193</v>
-      </c>
-      <c r="F12" s="33" t="s">
-        <v>217</v>
-      </c>
-      <c r="G12" s="33" t="s">
-        <v>202</v>
-      </c>
-      <c r="H12" s="33" t="s">
-        <v>178</v>
-      </c>
-      <c r="I12" s="33"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
+      <c r="H12" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="I12" s="28"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A13" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="H13" s="33"/>
-      <c r="I13" s="32"/>
+        <v>242</v>
+      </c>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="H13" s="28"/>
+      <c r="I13" s="27"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="G14" s="30" t="s">
-        <v>203</v>
-      </c>
-      <c r="H14" s="30">
+      <c r="G14" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="H14" s="25">
         <v>111111</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="G15" s="30"/>
+        <v>220</v>
+      </c>
+      <c r="G15" s="25"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A27" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A32" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A33" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A34" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A35" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A36" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A37" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -2441,8 +2444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A9AC7C-0DA4-46BC-A427-30A253EEB689}">
   <dimension ref="A1:AK13"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AK21" sqref="AK21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
@@ -2492,106 +2495,106 @@
         <v>41</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>104</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>80</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J1" s="11" t="s">
         <v>80</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M1" s="11" t="s">
         <v>80</v>
       </c>
       <c r="N1" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O1" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="P1" s="11" t="s">
         <v>80</v>
       </c>
       <c r="Q1" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R1" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S1" s="11" t="s">
         <v>80</v>
       </c>
       <c r="T1" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="U1" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="V1" s="11" t="s">
         <v>80</v>
       </c>
       <c r="W1" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="X1" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Y1" s="11" t="s">
         <v>80</v>
       </c>
       <c r="Z1" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA1" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AB1" s="11" t="s">
         <v>80</v>
       </c>
       <c r="AC1" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AD1" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AE1" s="11" t="s">
         <v>80</v>
       </c>
       <c r="AF1" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AG1" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AH1" s="11" t="s">
         <v>80</v>
       </c>
       <c r="AI1" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AJ1" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AK1" s="11" t="s">
         <v>80</v>
@@ -2716,7 +2719,7 @@
         <v>78</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="P3" s="12"/>
       <c r="Q3" s="1" t="s">
@@ -2833,7 +2836,7 @@
         <v>107</v>
       </c>
       <c r="AB4" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AC4" s="1" t="s">
         <v>106</v>
@@ -2872,7 +2875,7 @@
         <v>102</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>84</v>
@@ -2881,7 +2884,7 @@
         <v>102</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>84</v>
@@ -2890,7 +2893,7 @@
         <v>102</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>84</v>
@@ -2899,7 +2902,7 @@
         <v>102</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>84</v>
@@ -2908,7 +2911,7 @@
         <v>102</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>84</v>
@@ -2917,7 +2920,7 @@
         <v>102</v>
       </c>
       <c r="V5" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="W5" s="1" t="s">
         <v>84</v>
@@ -2926,7 +2929,7 @@
         <v>102</v>
       </c>
       <c r="Y5" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Z5" s="1" t="s">
         <v>84</v>
@@ -2935,7 +2938,7 @@
         <v>102</v>
       </c>
       <c r="AB5" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AC5" s="1" t="s">
         <v>84</v>
@@ -2944,7 +2947,7 @@
         <v>107</v>
       </c>
       <c r="AE5" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AF5" s="1" t="s">
         <v>84</v>
@@ -2953,7 +2956,7 @@
         <v>102</v>
       </c>
       <c r="AH5" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AI5" s="1" t="s">
         <v>84</v>
@@ -2962,12 +2965,12 @@
         <v>102</v>
       </c>
       <c r="AK5" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.5">
       <c r="B6" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>103</v>
@@ -2976,79 +2979,79 @@
         <v>105</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>103</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>103</v>
       </c>
       <c r="M6" s="12"/>
       <c r="N6" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="O6" s="10" t="s">
         <v>103</v>
       </c>
       <c r="P6" s="12"/>
       <c r="Q6" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="R6" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S6" s="12"/>
       <c r="T6" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U6" s="10" t="s">
         <v>103</v>
       </c>
       <c r="V6" s="12"/>
       <c r="W6" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="X6" s="10" t="s">
         <v>103</v>
       </c>
       <c r="Y6" s="12"/>
       <c r="Z6" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AA6" s="10" t="s">
         <v>103</v>
       </c>
       <c r="AB6" s="12"/>
       <c r="AC6" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AD6" s="10" t="s">
         <v>103</v>
       </c>
       <c r="AE6" s="12"/>
       <c r="AF6" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AG6" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AH6" s="12"/>
       <c r="AI6" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AJ6" s="10" t="s">
         <v>103</v>
@@ -3070,7 +3073,7 @@
         <v>107</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>87</v>
@@ -3079,7 +3082,7 @@
         <v>103</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>87</v>
@@ -3088,7 +3091,7 @@
         <v>107</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>87</v>
@@ -3097,7 +3100,7 @@
         <v>107</v>
       </c>
       <c r="P7" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>87</v>
@@ -3106,7 +3109,7 @@
         <v>107</v>
       </c>
       <c r="S7" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>87</v>
@@ -3115,7 +3118,7 @@
         <v>103</v>
       </c>
       <c r="V7" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="W7" s="1" t="s">
         <v>87</v>
@@ -3124,7 +3127,7 @@
         <v>107</v>
       </c>
       <c r="Y7" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Z7" s="1" t="s">
         <v>87</v>
@@ -3133,7 +3136,7 @@
         <v>107</v>
       </c>
       <c r="AB7" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AC7" s="1" t="s">
         <v>87</v>
@@ -3142,7 +3145,7 @@
         <v>103</v>
       </c>
       <c r="AE7" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AF7" s="1" t="s">
         <v>87</v>
@@ -3151,7 +3154,7 @@
         <v>107</v>
       </c>
       <c r="AH7" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AI7" s="1" t="s">
         <v>87</v>
@@ -3160,10 +3163,10 @@
         <v>107</v>
       </c>
       <c r="AK7" s="12" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.5">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" hidden="1" x14ac:dyDescent="0.5">
       <c r="B8" s="1" t="s">
         <v>89</v>
       </c>
@@ -3186,7 +3189,7 @@
         <v>89</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="1" t="s">
@@ -3196,7 +3199,7 @@
         <v>103</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>89</v>
@@ -3209,7 +3212,7 @@
         <v>89</v>
       </c>
       <c r="R8" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S8" s="12"/>
       <c r="T8" s="1" t="s">
@@ -3226,7 +3229,7 @@
         <v>103</v>
       </c>
       <c r="Y8" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Z8" s="1" t="s">
         <v>89</v>
@@ -3235,7 +3238,7 @@
         <v>103</v>
       </c>
       <c r="AB8" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AC8" s="1" t="s">
         <v>89</v>
@@ -3244,16 +3247,16 @@
         <v>103</v>
       </c>
       <c r="AE8" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AF8" s="1" t="s">
         <v>89</v>
       </c>
       <c r="AG8" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AH8" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AI8" s="1" t="s">
         <v>89</v>
@@ -3262,7 +3265,7 @@
         <v>103</v>
       </c>
       <c r="AK8" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.5">
@@ -3298,7 +3301,7 @@
         <v>107</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>91</v>
@@ -3385,14 +3388,14 @@
         <v>93</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M10" s="12"/>
       <c r="N10" s="1" t="s">
         <v>93</v>
       </c>
       <c r="O10" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P10" s="12"/>
       <c r="Q10" s="1" t="s">
@@ -3406,14 +3409,14 @@
         <v>93</v>
       </c>
       <c r="U10" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="V10" s="12"/>
       <c r="W10" s="1" t="s">
         <v>93</v>
       </c>
       <c r="X10" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="Y10" s="12"/>
       <c r="Z10" s="1" t="s">
@@ -3452,14 +3455,12 @@
       <c r="C11" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>110</v>
-      </c>
+      <c r="D11" s="12"/>
       <c r="E11" s="1" t="s">
         <v>94</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="1" t="s">
@@ -3473,14 +3474,14 @@
         <v>94</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M11" s="12"/>
       <c r="N11" s="1" t="s">
         <v>94</v>
       </c>
       <c r="O11" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P11" s="12"/>
       <c r="Q11" s="1" t="s">
@@ -3494,14 +3495,14 @@
         <v>94</v>
       </c>
       <c r="U11" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="V11" s="12"/>
       <c r="W11" s="1" t="s">
         <v>94</v>
       </c>
       <c r="X11" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Y11" s="12"/>
       <c r="Z11" s="1" t="s">
@@ -3538,14 +3539,14 @@
         <v>95</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="1" t="s">
         <v>95</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="1" t="s">
@@ -3559,14 +3560,14 @@
         <v>95</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M12" s="12"/>
       <c r="N12" s="1" t="s">
         <v>95</v>
       </c>
       <c r="O12" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P12" s="12"/>
       <c r="Q12" s="1" t="s">
@@ -3580,14 +3581,14 @@
         <v>95</v>
       </c>
       <c r="U12" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="V12" s="12"/>
       <c r="W12" s="1" t="s">
         <v>95</v>
       </c>
       <c r="X12" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Y12" s="12"/>
       <c r="Z12" s="1" t="s">
@@ -3624,7 +3625,7 @@
         <v>97</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="1" t="s">
@@ -3634,7 +3635,7 @@
         <v>103</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>97</v>
@@ -3643,7 +3644,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>97</v>
@@ -3652,7 +3653,7 @@
         <v>103</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>97</v>
@@ -3661,7 +3662,7 @@
         <v>103</v>
       </c>
       <c r="P13" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q13" s="1" t="s">
         <v>97</v>
@@ -3670,16 +3671,16 @@
         <v>103</v>
       </c>
       <c r="S13" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="T13" s="1" t="s">
         <v>97</v>
       </c>
       <c r="U13" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="V13" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="W13" s="1" t="s">
         <v>97</v>
@@ -3688,7 +3689,7 @@
         <v>103</v>
       </c>
       <c r="Y13" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Z13" s="1" t="s">
         <v>97</v>
@@ -3697,7 +3698,7 @@
         <v>103</v>
       </c>
       <c r="AB13" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AC13" s="1" t="s">
         <v>97</v>
@@ -3706,7 +3707,7 @@
         <v>103</v>
       </c>
       <c r="AE13" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AF13" s="1" t="s">
         <v>97</v>
@@ -3715,16 +3716,16 @@
         <v>103</v>
       </c>
       <c r="AH13" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AI13" s="1" t="s">
         <v>97</v>
       </c>
       <c r="AJ13" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AK13" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -3734,10 +3735,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD505EFA-7D11-43A5-AB74-E1417C081A89}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
@@ -3762,10 +3763,10 @@
         <v>80</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.5">
@@ -3776,16 +3777,16 @@
         <v>81</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E2" s="22">
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.5">
@@ -3796,16 +3797,19 @@
         <v>82</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E3" s="22">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.5">
@@ -3822,7 +3826,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.5">
@@ -3839,15 +3843,15 @@
         <v>2</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6" s="24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>86</v>
@@ -3862,13 +3866,13 @@
         <v>4</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.5">
@@ -3885,13 +3889,13 @@
         <v>4</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.5">
@@ -3940,6 +3944,11 @@
       </c>
       <c r="B13" s="21" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B19" s="1" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -4198,191 +4207,204 @@
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="26" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="28"/>
-      <c r="J2" s="26" t="s">
+      <c r="I2" s="32"/>
+      <c r="J2" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="28"/>
-      <c r="L2" s="26" t="s">
+      <c r="K2" s="32"/>
+      <c r="L2" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="28"/>
-      <c r="N2" s="26" t="s">
+      <c r="M2" s="32"/>
+      <c r="N2" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="28"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="32"/>
       <c r="V2" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="26" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="28"/>
-      <c r="J3" s="26" t="s">
+      <c r="I3" s="32"/>
+      <c r="J3" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="28"/>
-      <c r="L3" s="26" t="s">
+      <c r="K3" s="32"/>
+      <c r="L3" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="27"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="U3" s="28"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="32"/>
       <c r="V3" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="26" t="s">
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="28"/>
-      <c r="J4" s="26" t="s">
+      <c r="I4" s="32"/>
+      <c r="J4" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="28"/>
-      <c r="L4" s="26" t="s">
+      <c r="K4" s="32"/>
+      <c r="L4" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="27"/>
-      <c r="S4" s="27"/>
-      <c r="T4" s="27"/>
-      <c r="U4" s="28"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="32"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="26" t="s">
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="28"/>
-      <c r="J5" s="26" t="s">
+      <c r="I5" s="32"/>
+      <c r="J5" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="28"/>
-      <c r="L5" s="26" t="s">
+      <c r="K5" s="32"/>
+      <c r="L5" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="27"/>
-      <c r="S5" s="27"/>
-      <c r="T5" s="27"/>
-      <c r="U5" s="28"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="32"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="26" t="s">
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="28"/>
-      <c r="J6" s="26" t="s">
+      <c r="I6" s="32"/>
+      <c r="J6" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="27"/>
-      <c r="R6" s="27"/>
-      <c r="S6" s="27"/>
-      <c r="T6" s="27"/>
-      <c r="U6" s="28"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="31"/>
+      <c r="T6" s="31"/>
+      <c r="U6" s="32"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="26" t="s">
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="28"/>
-      <c r="S7" s="26" t="s">
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="T7" s="27"/>
-      <c r="U7" s="28"/>
+      <c r="T7" s="31"/>
+      <c r="U7" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:U2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:U3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:U4"/>
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="H7:R7"/>
     <mergeCell ref="S7:U7"/>
@@ -4393,19 +4415,6 @@
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="J6:U6"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:U3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:U4"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:U2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished Roughly half of multicycle
</commit_message>
<xml_diff>
--- a/materials/Instructions.xlsx
+++ b/materials/Instructions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingi\Documents\UTD\4310 Arch\Project\materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF13251-945A-4711-88E8-905ED61C22A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF9F8C3-D715-4B51-805A-A7301B1F3EF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="797" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction Types" sheetId="1" r:id="rId1"/>
@@ -100,8 +100,43 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Stephen Campbell</author>
+  </authors>
+  <commentList>
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{0D747D89-C2E7-4002-85FB-1EBCBC478619}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="22"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Stephen Campbell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="22"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Not needed because jump address covers all bits
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="298">
   <si>
     <t>Opcode</t>
   </si>
@@ -862,15 +897,6 @@
     <t>control (opcode)</t>
   </si>
   <si>
-    <t>regFile selA</t>
-  </si>
-  <si>
-    <t>regFile selB</t>
-  </si>
-  <si>
-    <t>regFile selWrite</t>
-  </si>
-  <si>
     <t>regWriteDestMux</t>
   </si>
   <si>
@@ -919,12 +945,6 @@
     <t>Memory (address)</t>
   </si>
   <si>
-    <t xml:space="preserve">pcWrite </t>
-  </si>
-  <si>
-    <t>Control (pcwrite &amp; pcWriteCond)</t>
-  </si>
-  <si>
     <t>Control (memGetData)</t>
   </si>
   <si>
@@ -934,9 +954,6 @@
     <t>Memory (isReading)</t>
   </si>
   <si>
-    <t>Control (regWriteDataSel)</t>
-  </si>
-  <si>
     <t>Control (IR write)</t>
   </si>
   <si>
@@ -956,13 +973,70 @@
   </si>
   <si>
     <t>Control (PCsrc)</t>
+  </si>
+  <si>
+    <t>pcWriteCombo</t>
+  </si>
+  <si>
+    <t>ADDRESS_SIZE</t>
+  </si>
+  <si>
+    <t>WORD_SIZE</t>
+  </si>
+  <si>
+    <t>OPCODE_SIZE</t>
+  </si>
+  <si>
+    <t>REG_ADDRESS_SIZE</t>
+  </si>
+  <si>
+    <t>1 bit</t>
+  </si>
+  <si>
+    <t>Control (pcwrite )</t>
+  </si>
+  <si>
+    <t>Control (pcwriteCond )</t>
+  </si>
+  <si>
+    <t>2 bits</t>
+  </si>
+  <si>
+    <t>4 bits</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>JUMP_ADDRESS_SIZE</t>
+  </si>
+  <si>
+    <t>BIG_IMMEDIATE_SIZE</t>
+  </si>
+  <si>
+    <t>SMALL_IMMEDIATE_SIZE</t>
+  </si>
+  <si>
+    <t>1bit</t>
+  </si>
+  <si>
+    <t>Control (regWriteDataSelect)</t>
+  </si>
+  <si>
+    <t>regFile selAlpha</t>
+  </si>
+  <si>
+    <t>regFile selBeta</t>
+  </si>
+  <si>
+    <t>regFile selGamma (write)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1020,8 +1094,21 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1037,6 +1124,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1145,7 +1238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1208,6 +1301,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1488,10 +1584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U14"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10:U10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11:U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
@@ -1736,6 +1832,351 @@
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="27"/>
+      <c r="Q16" s="27"/>
+      <c r="R16" s="27"/>
+      <c r="S16" s="27"/>
+      <c r="T16" s="27"/>
+      <c r="U16" s="27"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A17" s="26"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="38"/>
+      <c r="R17" s="38"/>
+      <c r="S17" s="38"/>
+      <c r="T17" s="38"/>
+      <c r="U17" s="38"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="27"/>
+      <c r="R18" s="27"/>
+      <c r="S18" s="27"/>
+      <c r="T18" s="27"/>
+      <c r="U18" s="27"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A19" s="26"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="38"/>
+      <c r="P19" s="38"/>
+      <c r="Q19" s="38"/>
+      <c r="R19" s="38"/>
+      <c r="S19" s="38"/>
+      <c r="T19" s="38"/>
+      <c r="U19" s="38"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="27"/>
+      <c r="Q20" s="27"/>
+      <c r="R20" s="27"/>
+      <c r="S20" s="27"/>
+      <c r="T20" s="27"/>
+      <c r="U20" s="27"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A21" s="26"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="38"/>
+      <c r="O21" s="38"/>
+      <c r="P21" s="38"/>
+      <c r="Q21" s="38"/>
+      <c r="R21" s="38"/>
+      <c r="S21" s="38"/>
+      <c r="T21" s="38"/>
+      <c r="U21" s="38"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="27"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="27"/>
+      <c r="Q22" s="27"/>
+      <c r="R22" s="27"/>
+      <c r="S22" s="27"/>
+      <c r="T22" s="27"/>
+      <c r="U22" s="27"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="27"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="27"/>
+      <c r="Q23" s="27"/>
+      <c r="R23" s="27"/>
+      <c r="S23" s="27"/>
+      <c r="T23" s="27"/>
+      <c r="U23" s="27"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A24" s="26"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="38"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="38"/>
+      <c r="P24" s="38"/>
+      <c r="Q24" s="38"/>
+      <c r="R24" s="38"/>
+      <c r="S24" s="38"/>
+      <c r="T24" s="38"/>
+      <c r="U24" s="38"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A25" s="27"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="38"/>
+      <c r="R25" s="38"/>
+      <c r="S25" s="38"/>
+      <c r="T25" s="38"/>
+      <c r="U25" s="38"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A26" s="27"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="27"/>
+      <c r="N26" s="27"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="27"/>
+      <c r="Q26" s="27"/>
+      <c r="R26" s="27"/>
+      <c r="S26" s="27"/>
+      <c r="T26" s="27"/>
+      <c r="U26" s="27"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A27" s="26"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="38"/>
+      <c r="L27" s="38"/>
+      <c r="M27" s="38"/>
+      <c r="N27" s="38"/>
+      <c r="O27" s="38"/>
+      <c r="P27" s="38"/>
+      <c r="Q27" s="38"/>
+      <c r="R27" s="38"/>
+      <c r="S27" s="38"/>
+      <c r="T27" s="38"/>
+      <c r="U27" s="38"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="27"/>
+      <c r="M28" s="27"/>
+      <c r="N28" s="27"/>
+      <c r="O28" s="27"/>
+      <c r="P28" s="27"/>
+      <c r="Q28" s="27"/>
+      <c r="R28" s="27"/>
+      <c r="S28" s="27"/>
+      <c r="T28" s="27"/>
+      <c r="U28" s="27"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A29" s="26"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="38"/>
+      <c r="M29" s="38"/>
+      <c r="N29" s="38"/>
+      <c r="O29" s="38"/>
+      <c r="P29" s="38"/>
+      <c r="Q29" s="38"/>
+      <c r="R29" s="38"/>
+      <c r="S29" s="38"/>
+      <c r="T29" s="38"/>
+      <c r="U29" s="38"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="27"/>
+      <c r="M30" s="27"/>
+      <c r="N30" s="27"/>
+      <c r="O30" s="27"/>
+      <c r="P30" s="27"/>
+      <c r="Q30" s="27"/>
+      <c r="R30" s="27"/>
+      <c r="S30" s="27"/>
+      <c r="T30" s="27"/>
+      <c r="U30" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="23">
@@ -1773,7 +2214,7 @@
   <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.5" x14ac:dyDescent="0.45"/>
@@ -3855,21 +4296,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EAB20A-8932-4835-BF8E-F6B57D7CCDEF}">
-  <dimension ref="A1:C43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EAB20A-8932-4835-BF8E-F6B57D7CCDEF}">
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="67.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="73.7109375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="52.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>246</v>
       </c>
@@ -3877,10 +4320,13 @@
         <v>247</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+        <v>267</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>67</v>
       </c>
@@ -3890,8 +4336,11 @@
       <c r="C2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D2" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>67</v>
       </c>
@@ -3901,453 +4350,619 @@
       <c r="C3" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A4" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A4" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="36" t="s">
         <v>249</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="36">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D4" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>250</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="37">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D5" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>250</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="37">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D6" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>251</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="37">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D7" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>251</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="C8" s="1">
+        <v>256</v>
+      </c>
+      <c r="C8" s="37">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D8" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>251</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="C9" s="1">
+        <v>295</v>
+      </c>
+      <c r="C9" s="37">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D9" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>251</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="C10" s="1">
+        <v>296</v>
+      </c>
+      <c r="C10" s="37">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D10" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>251</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="C11" s="1">
+        <v>297</v>
+      </c>
+      <c r="C11" s="37">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D11" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>251</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="C12" s="1">
+        <v>265</v>
+      </c>
+      <c r="C12" s="37">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D12" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>251</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="C13" s="1">
+        <v>266</v>
+      </c>
+      <c r="C13" s="37">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D13" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>166</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C14" s="1">
+        <v>253</v>
+      </c>
+      <c r="C14" s="37">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D14" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C15" s="37">
+        <v>14</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A16" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="C15" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A16" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C16" s="1">
+      <c r="C16" s="37">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D16" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="37">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D17" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C18" s="37">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A19" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C19" s="37">
+        <v>18</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A20" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="C18" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A19" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="C19" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A20" s="1" t="s">
-        <v>260</v>
-      </c>
       <c r="B20" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="C20" s="1">
+        <v>254</v>
+      </c>
+      <c r="C20" s="37">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D20" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A21" s="25">
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="C21" s="1">
+        <v>254</v>
+      </c>
+      <c r="C21" s="37">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D21" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>248</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="C22" s="1">
+        <v>261</v>
+      </c>
+      <c r="C22" s="37">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D22" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="C23" s="1">
+        <v>262</v>
+      </c>
+      <c r="C23" s="37">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D23" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="37">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D24" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="C25" s="1">
+        <v>279</v>
+      </c>
+      <c r="C25" s="37">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D25" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="37">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D26" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A27" s="1" t="s">
-        <v>149</v>
+        <v>256</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="37">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D27" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
         <v>149</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="C28" s="1">
+        <v>249</v>
+      </c>
+      <c r="C28" s="37">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D28" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
         <v>149</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C29" s="1">
+        <v>264</v>
+      </c>
+      <c r="C29" s="37">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D29" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C30" s="37">
+        <v>29</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A31" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C31" s="37">
+        <v>30</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A32" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="37">
+        <v>31</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A33" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C30" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A31" s="1" t="s">
+      <c r="C33" s="37">
+        <v>32</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C34" s="37">
+        <v>33</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A35" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C35" s="37">
+        <v>34</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A36" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C36" s="37">
+        <v>35</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A37" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C37" s="37">
+        <v>36</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A38" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C38" s="37">
+        <v>37</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A39" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C39" s="37">
+        <v>38</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A40" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C40" s="37">
+        <v>39</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A41" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C41" s="37">
+        <v>40</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A42" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C42" s="37">
+        <v>41</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A43" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C43" s="37">
+        <v>42</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A44" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C44" s="37">
+        <v>43</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A45" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C45" s="37">
+        <v>44</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A46" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A32" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="C32" s="1">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A33" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="C33" s="1">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A34" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="C34" s="1">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A35" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="C35" s="1">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A36" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="C36" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A37" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C37" s="1">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A38" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="C38" s="1">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A39" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="C39" s="1">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A40" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="C40" s="1">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A41" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="C41" s="1">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A42" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="C42" s="1">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A43" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="C43" s="1">
-        <v>42</v>
+      <c r="C46" s="1">
+        <v>45</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>293</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C33">
-    <sortCondition ref="C2:C33"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C34">
+    <sortCondition ref="C2:C34"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4356,7 +4971,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
Added Load instruction to  Memory File and made RAM async because we already have the instruction register
</commit_message>
<xml_diff>
--- a/materials/Instructions.xlsx
+++ b/materials/Instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingi\Documents\UTD\4310 Arch\Project\materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CB1977-5045-41E8-8934-B20DFEC0DB2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038CD5E2-D9E9-43D4-9CCB-BB7858FCC619}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="797" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="318">
   <si>
     <t>Opcode</t>
   </si>
@@ -1087,6 +1087,9 @@
   </si>
   <si>
     <t>regFile Write data</t>
+  </si>
+  <si>
+    <t>RT</t>
   </si>
 </sst>
 </file>
@@ -1337,6 +1340,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1358,9 +1364,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1644,7 +1647,7 @@
   <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
@@ -1658,36 +1661,36 @@
       <c r="A1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29" t="s">
+      <c r="I1" s="32"/>
+      <c r="J1" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29" t="s">
+      <c r="K1" s="32"/>
+      <c r="L1" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="29"/>
-      <c r="N1" s="30" t="s">
+      <c r="M1" s="32"/>
+      <c r="N1" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="32"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="35"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
@@ -1698,34 +1701,34 @@
       <c r="A3" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29" t="s">
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29" t="s">
+      <c r="I3" s="32"/>
+      <c r="J3" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="29"/>
-      <c r="L3" s="30" t="s">
+      <c r="K3" s="32"/>
+      <c r="L3" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="31"/>
-      <c r="S3" s="31"/>
-      <c r="T3" s="31"/>
-      <c r="U3" s="32"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="34"/>
+      <c r="S3" s="34"/>
+      <c r="T3" s="34"/>
+      <c r="U3" s="35"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
@@ -1736,34 +1739,34 @@
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="30" t="s">
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="32"/>
-      <c r="J5" s="30" t="s">
+      <c r="I5" s="35"/>
+      <c r="J5" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="32"/>
-      <c r="L5" s="30" t="s">
+      <c r="K5" s="35"/>
+      <c r="L5" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="31"/>
-      <c r="T5" s="31"/>
-      <c r="U5" s="32"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="34"/>
+      <c r="U5" s="35"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
@@ -1779,39 +1782,67 @@
       <c r="A8" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="32"/>
-      <c r="J8" s="30" t="s">
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="32"/>
-      <c r="L8" s="30" t="s">
+      <c r="I8" s="35"/>
+      <c r="J8" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="K8" s="35"/>
+      <c r="L8" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="31"/>
-      <c r="T8" s="31"/>
-      <c r="U8" s="32"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="34"/>
+      <c r="Q8" s="34"/>
+      <c r="R8" s="34"/>
+      <c r="S8" s="34"/>
+      <c r="T8" s="34"/>
+      <c r="U8" s="35"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="B9" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="35"/>
+      <c r="J9" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="35"/>
+      <c r="L9" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="34"/>
+      <c r="S9" s="34"/>
+      <c r="T9" s="34"/>
+      <c r="U9" s="35"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
@@ -1822,32 +1853,32 @@
       <c r="A11" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="30" t="s">
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I11" s="32"/>
-      <c r="J11" s="30" t="s">
+      <c r="I11" s="35"/>
+      <c r="J11" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="31"/>
-      <c r="R11" s="31"/>
-      <c r="S11" s="31"/>
-      <c r="T11" s="31"/>
-      <c r="U11" s="32"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34"/>
+      <c r="S11" s="34"/>
+      <c r="T11" s="34"/>
+      <c r="U11" s="35"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
@@ -1858,32 +1889,32 @@
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="30" t="s">
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="30" t="s">
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="35"/>
+      <c r="Q13" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="R13" s="31"/>
-      <c r="S13" s="31"/>
-      <c r="T13" s="31"/>
-      <c r="U13" s="32"/>
+      <c r="R13" s="34"/>
+      <c r="S13" s="34"/>
+      <c r="T13" s="34"/>
+      <c r="U13" s="35"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
@@ -1915,26 +1946,26 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A17" s="26"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
-      <c r="L17" s="38"/>
-      <c r="M17" s="38"/>
-      <c r="N17" s="38"/>
-      <c r="O17" s="38"/>
-      <c r="P17" s="38"/>
-      <c r="Q17" s="38"/>
-      <c r="R17" s="38"/>
-      <c r="S17" s="38"/>
-      <c r="T17" s="38"/>
-      <c r="U17" s="38"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
+      <c r="P17" s="31"/>
+      <c r="Q17" s="31"/>
+      <c r="R17" s="31"/>
+      <c r="S17" s="31"/>
+      <c r="T17" s="31"/>
+      <c r="U17" s="31"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A18" s="27"/>
@@ -1963,33 +1994,33 @@
       <c r="A19" s="26" t="s">
         <v>293</v>
       </c>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="38"/>
-      <c r="M19" s="38"/>
-      <c r="N19" s="38"/>
-      <c r="O19" s="38"/>
-      <c r="P19" s="38"/>
-      <c r="Q19" s="38"/>
-      <c r="R19" s="38"/>
-      <c r="S19" s="38"/>
-      <c r="T19" s="38"/>
-      <c r="U19" s="38"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="31"/>
+      <c r="Q19" s="31"/>
+      <c r="R19" s="31"/>
+      <c r="S19" s="31"/>
+      <c r="T19" s="31"/>
+      <c r="U19" s="31"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A20" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="31" t="s">
         <v>294</v>
       </c>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="31" t="s">
         <v>297</v>
       </c>
       <c r="D20" s="27"/>
@@ -2021,33 +2052,33 @@
       <c r="C21" s="27">
         <v>1</v>
       </c>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="38"/>
-      <c r="L21" s="38"/>
-      <c r="M21" s="38"/>
-      <c r="N21" s="38"/>
-      <c r="O21" s="38"/>
-      <c r="P21" s="38"/>
-      <c r="Q21" s="38"/>
-      <c r="R21" s="38"/>
-      <c r="S21" s="38"/>
-      <c r="T21" s="38"/>
-      <c r="U21" s="38"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="31"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="31"/>
+      <c r="Q21" s="31"/>
+      <c r="R21" s="31"/>
+      <c r="S21" s="31"/>
+      <c r="T21" s="31"/>
+      <c r="U21" s="31"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A22" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="31" t="s">
         <v>296</v>
       </c>
-      <c r="C22" s="38">
+      <c r="C22" s="31">
         <v>2</v>
       </c>
       <c r="D22" s="27"/>
@@ -2098,58 +2129,58 @@
       <c r="A24" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="38"/>
-      <c r="L24" s="38"/>
-      <c r="M24" s="38"/>
-      <c r="N24" s="38"/>
-      <c r="O24" s="38"/>
-      <c r="P24" s="38"/>
-      <c r="Q24" s="38"/>
-      <c r="R24" s="38"/>
-      <c r="S24" s="38"/>
-      <c r="T24" s="38"/>
-      <c r="U24" s="38"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="31"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="31"/>
+      <c r="R24" s="31"/>
+      <c r="S24" s="31"/>
+      <c r="T24" s="31"/>
+      <c r="U24" s="31"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A25" s="27"/>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="38"/>
-      <c r="L25" s="38"/>
-      <c r="M25" s="38"/>
-      <c r="N25" s="38"/>
-      <c r="O25" s="38"/>
-      <c r="P25" s="38"/>
-      <c r="Q25" s="38"/>
-      <c r="R25" s="38"/>
-      <c r="S25" s="38"/>
-      <c r="T25" s="38"/>
-      <c r="U25" s="38"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="31"/>
+      <c r="O25" s="31"/>
+      <c r="P25" s="31"/>
+      <c r="Q25" s="31"/>
+      <c r="R25" s="31"/>
+      <c r="S25" s="31"/>
+      <c r="T25" s="31"/>
+      <c r="U25" s="31"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A26" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="B26" s="38" t="s">
+      <c r="B26" s="31" t="s">
         <v>294</v>
       </c>
-      <c r="C26" s="38">
+      <c r="C26" s="31">
         <v>1</v>
       </c>
       <c r="D26" s="27"/>
@@ -2181,33 +2212,33 @@
       <c r="C27" s="27">
         <v>2</v>
       </c>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="38"/>
-      <c r="N27" s="38"/>
-      <c r="O27" s="38"/>
-      <c r="P27" s="38"/>
-      <c r="Q27" s="38"/>
-      <c r="R27" s="38"/>
-      <c r="S27" s="38"/>
-      <c r="T27" s="38"/>
-      <c r="U27" s="38"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="31"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="31"/>
+      <c r="O27" s="31"/>
+      <c r="P27" s="31"/>
+      <c r="Q27" s="31"/>
+      <c r="R27" s="31"/>
+      <c r="S27" s="31"/>
+      <c r="T27" s="31"/>
+      <c r="U27" s="31"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A28" s="27" t="s">
         <v>302</v>
       </c>
-      <c r="B28" s="38" t="s">
+      <c r="B28" s="31" t="s">
         <v>296</v>
       </c>
-      <c r="C28" s="38"/>
+      <c r="C28" s="31"/>
       <c r="D28" s="27"/>
       <c r="E28" s="27" t="s">
         <v>303</v>
@@ -2233,29 +2264,29 @@
       <c r="A29" s="27"/>
       <c r="B29" s="27"/>
       <c r="C29" s="27"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
-      <c r="K29" s="38"/>
-      <c r="L29" s="38"/>
-      <c r="M29" s="38"/>
-      <c r="N29" s="38"/>
-      <c r="O29" s="38"/>
-      <c r="P29" s="38"/>
-      <c r="Q29" s="38"/>
-      <c r="R29" s="38"/>
-      <c r="S29" s="38"/>
-      <c r="T29" s="38"/>
-      <c r="U29" s="38"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="31"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="31"/>
+      <c r="P29" s="31"/>
+      <c r="Q29" s="31"/>
+      <c r="R29" s="31"/>
+      <c r="S29" s="31"/>
+      <c r="T29" s="31"/>
+      <c r="U29" s="31"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A30" s="27"/>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
       <c r="F30" s="27"/>
@@ -2276,12 +2307,15 @@
       <c r="U30" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:U1"/>
+  <mergeCells count="27">
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:U3"/>
+    <mergeCell ref="L5:U5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B5:G5"/>
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="B8:G8"/>
     <mergeCell ref="H8:I8"/>
@@ -2292,14 +2326,15 @@
     <mergeCell ref="J11:U11"/>
     <mergeCell ref="Q13:U13"/>
     <mergeCell ref="H13:P13"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:U3"/>
-    <mergeCell ref="L5:U5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:U9"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2353,26 +2388,26 @@
       <c r="A2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
     </row>
     <row r="3" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
       <c r="G3" s="6" t="s">
         <v>130</v>
       </c>
@@ -2402,10 +2437,10 @@
       <c r="A5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="C5" s="35"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
         <v>63</v>
@@ -2518,23 +2553,23 @@
       <c r="A47" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B47" s="33" t="s">
+      <c r="B47" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="C47" s="33"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="33"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="36"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B48" s="33" t="s">
+      <c r="B48" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="C48" s="33"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="33"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="36"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" s="5" t="s">
@@ -2595,23 +2630,23 @@
       <c r="A54" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B54" s="33" t="s">
+      <c r="B54" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="C54" s="33"/>
-      <c r="D54" s="33"/>
-      <c r="E54" s="33"/>
+      <c r="C54" s="36"/>
+      <c r="D54" s="36"/>
+      <c r="E54" s="36"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B55" s="33" t="s">
+      <c r="B55" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="C55" s="33"/>
-      <c r="D55" s="33"/>
-      <c r="E55" s="33"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="36"/>
+      <c r="E55" s="36"/>
     </row>
     <row r="56" spans="1:5" ht="57" x14ac:dyDescent="0.45">
       <c r="A56" s="5" t="s">
@@ -2702,8 +2737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E23297D-859B-4DF0-AD52-FCC5F95569EC}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
@@ -4396,8 +4431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EAB20A-8932-4835-BF8E-F6B57D7CCDEF}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
@@ -4424,16 +4459,16 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="29" t="s">
         <v>245</v>
       </c>
-      <c r="C2" s="36">
+      <c r="C2" s="29">
         <v>1</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="29" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4452,16 +4487,16 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="29" t="s">
         <v>249</v>
       </c>
-      <c r="C4" s="36">
+      <c r="C4" s="29">
         <v>3</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="29" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4472,7 +4507,7 @@
       <c r="B5" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C5" s="37">
+      <c r="C5" s="30">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -4486,7 +4521,7 @@
       <c r="B6" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C6" s="37">
+      <c r="C6" s="30">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -4500,7 +4535,7 @@
       <c r="B7" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C7" s="37">
+      <c r="C7" s="30">
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -4514,7 +4549,7 @@
       <c r="B8" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C8" s="37">
+      <c r="C8" s="30">
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -4528,7 +4563,7 @@
       <c r="B9" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C9" s="37">
+      <c r="C9" s="30">
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -4542,7 +4577,7 @@
       <c r="B10" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="C10" s="37">
+      <c r="C10" s="30">
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -4556,7 +4591,7 @@
       <c r="B11" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="C11" s="37">
+      <c r="C11" s="30">
         <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -4570,7 +4605,7 @@
       <c r="B12" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="C12" s="37">
+      <c r="C12" s="30">
         <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -4584,7 +4619,7 @@
       <c r="B13" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="C13" s="37">
+      <c r="C13" s="30">
         <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -4598,7 +4633,7 @@
       <c r="B14" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="C14" s="37">
+      <c r="C14" s="30">
         <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -4612,7 +4647,7 @@
       <c r="B15" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="C15" s="37">
+      <c r="C15" s="30">
         <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -4626,7 +4661,7 @@
       <c r="B16" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C16" s="37">
+      <c r="C16" s="30">
         <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -4640,7 +4675,7 @@
       <c r="B17" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="C17" s="37">
+      <c r="C17" s="30">
         <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -4654,7 +4689,7 @@
       <c r="B18" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C18" s="37">
+      <c r="C18" s="30">
         <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -4668,7 +4703,7 @@
       <c r="B19" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C19" s="37">
+      <c r="C19" s="30">
         <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -4677,12 +4712,12 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C20" s="37">
+      <c r="C20" s="30">
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -4696,7 +4731,7 @@
       <c r="B21" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C21" s="37">
+      <c r="C21" s="30">
         <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -4710,7 +4745,7 @@
       <c r="B22" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C22" s="37">
+      <c r="C22" s="30">
         <v>21</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -4724,7 +4759,7 @@
       <c r="B23" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C23" s="37">
+      <c r="C23" s="30">
         <v>22</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -4738,7 +4773,7 @@
       <c r="B24" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C24" s="37">
+      <c r="C24" s="30">
         <v>23</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -4752,7 +4787,7 @@
       <c r="B25" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C25" s="37">
+      <c r="C25" s="30">
         <v>24</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -4766,7 +4801,7 @@
       <c r="B26" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="C26" s="37">
+      <c r="C26" s="30">
         <v>25</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -4780,7 +4815,7 @@
       <c r="B27" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C27" s="37">
+      <c r="C27" s="30">
         <v>26</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -4794,7 +4829,7 @@
       <c r="B28" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C28" s="37">
+      <c r="C28" s="30">
         <v>27</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -4808,7 +4843,7 @@
       <c r="B29" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C29" s="37">
+      <c r="C29" s="30">
         <v>28</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -4822,7 +4857,7 @@
       <c r="B30" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C30" s="37">
+      <c r="C30" s="30">
         <v>29</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -4836,7 +4871,7 @@
       <c r="B31" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="C31" s="37">
+      <c r="C31" s="30">
         <v>30</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -4850,7 +4885,7 @@
       <c r="B32" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="C32" s="37">
+      <c r="C32" s="30">
         <v>31</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -4864,7 +4899,7 @@
       <c r="B33" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="37">
+      <c r="C33" s="30">
         <v>32</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -4878,7 +4913,7 @@
       <c r="B34" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="C34" s="37">
+      <c r="C34" s="30">
         <v>33</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -4892,7 +4927,7 @@
       <c r="B35" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="C35" s="37">
+      <c r="C35" s="30">
         <v>34</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -4906,7 +4941,7 @@
       <c r="B36" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="C36" s="37">
+      <c r="C36" s="30">
         <v>35</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -4920,7 +4955,7 @@
       <c r="B37" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C37" s="37">
+      <c r="C37" s="30">
         <v>36</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -4934,7 +4969,7 @@
       <c r="B38" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="C38" s="37">
+      <c r="C38" s="30">
         <v>37</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -4948,7 +4983,7 @@
       <c r="B39" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="C39" s="37">
+      <c r="C39" s="30">
         <v>38</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -4962,7 +4997,7 @@
       <c r="B40" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C40" s="37">
+      <c r="C40" s="30">
         <v>39</v>
       </c>
       <c r="D40" s="1" t="s">
@@ -4976,7 +5011,7 @@
       <c r="B41" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="C41" s="37">
+      <c r="C41" s="30">
         <v>40</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -4990,7 +5025,7 @@
       <c r="B42" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C42" s="37">
+      <c r="C42" s="30">
         <v>41</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -5004,7 +5039,7 @@
       <c r="B43" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C43" s="37">
+      <c r="C43" s="30">
         <v>42</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -5018,7 +5053,7 @@
       <c r="B44" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C44" s="37">
+      <c r="C44" s="30">
         <v>43</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -5032,7 +5067,7 @@
       <c r="B45" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C45" s="37">
+      <c r="C45" s="30">
         <v>44</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -5046,7 +5081,7 @@
       <c r="B46" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="C46" s="37">
+      <c r="C46" s="30">
         <v>45</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -5060,7 +5095,7 @@
       <c r="B47" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C47" s="37">
+      <c r="C47" s="30">
         <v>46</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -5074,7 +5109,7 @@
       <c r="B48" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="C48" s="37">
+      <c r="C48" s="30">
         <v>47</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -5088,7 +5123,7 @@
       <c r="B49" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C49" s="37">
+      <c r="C49" s="30">
         <v>48</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -5102,7 +5137,7 @@
       <c r="B50" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="C50" s="37">
+      <c r="C50" s="30">
         <v>49</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -5116,7 +5151,7 @@
       <c r="B51" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="C51" s="37">
+      <c r="C51" s="30">
         <v>50</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -5138,7 +5173,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
@@ -5448,7 +5483,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5607,204 +5642,191 @@
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="30" t="s">
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="32"/>
-      <c r="J2" s="30" t="s">
+      <c r="I2" s="35"/>
+      <c r="J2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="30" t="s">
+      <c r="K2" s="35"/>
+      <c r="L2" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="32"/>
-      <c r="N2" s="30" t="s">
+      <c r="M2" s="35"/>
+      <c r="N2" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="32"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="35"/>
       <c r="V2" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="30" t="s">
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="30" t="s">
+      <c r="I3" s="35"/>
+      <c r="J3" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="32"/>
-      <c r="L3" s="30" t="s">
+      <c r="K3" s="35"/>
+      <c r="L3" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="31"/>
-      <c r="S3" s="31"/>
-      <c r="T3" s="31"/>
-      <c r="U3" s="32"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="34"/>
+      <c r="S3" s="34"/>
+      <c r="T3" s="34"/>
+      <c r="U3" s="35"/>
       <c r="V3" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="30" t="s">
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="32"/>
-      <c r="J4" s="30" t="s">
+      <c r="I4" s="35"/>
+      <c r="J4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="32"/>
-      <c r="L4" s="30" t="s">
+      <c r="K4" s="35"/>
+      <c r="L4" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="31"/>
-      <c r="R4" s="31"/>
-      <c r="S4" s="31"/>
-      <c r="T4" s="31"/>
-      <c r="U4" s="32"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="34"/>
+      <c r="S4" s="34"/>
+      <c r="T4" s="34"/>
+      <c r="U4" s="35"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="30" t="s">
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="32"/>
-      <c r="J5" s="30" t="s">
+      <c r="I5" s="35"/>
+      <c r="J5" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="32"/>
-      <c r="L5" s="30" t="s">
+      <c r="K5" s="35"/>
+      <c r="L5" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="31"/>
-      <c r="T5" s="31"/>
-      <c r="U5" s="32"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="34"/>
+      <c r="U5" s="35"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="30" t="s">
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="32"/>
-      <c r="J6" s="30" t="s">
+      <c r="I6" s="35"/>
+      <c r="J6" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="31"/>
-      <c r="S6" s="31"/>
-      <c r="T6" s="31"/>
-      <c r="U6" s="32"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="34"/>
+      <c r="S6" s="34"/>
+      <c r="T6" s="34"/>
+      <c r="U6" s="35"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.5">
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="30" t="s">
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="32"/>
-      <c r="S7" s="30" t="s">
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="35"/>
+      <c r="S7" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="T7" s="31"/>
-      <c r="U7" s="32"/>
+      <c r="T7" s="34"/>
+      <c r="U7" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:U2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:U3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:U4"/>
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="H7:R7"/>
     <mergeCell ref="S7:U7"/>
@@ -5815,6 +5837,19 @@
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="J6:U6"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:U3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:U4"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:U2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Renamed mem and data for add progam to allow other programs.
</commit_message>
<xml_diff>
--- a/materials/Instructions.xlsx
+++ b/materials/Instructions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingi\Documents\UTD\4310 Arch\Project\materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038CD5E2-D9E9-43D4-9CCB-BB7858FCC619}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756DDD9C-7841-4BE6-A7B8-CFA2D2E8CB36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="797" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="797" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction Types" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="320">
   <si>
     <t>Opcode</t>
   </si>
@@ -867,9 +867,6 @@
     <t>Opcodes</t>
   </si>
   <si>
-    <t>kk</t>
-  </si>
-  <si>
     <t>SE imm_big</t>
   </si>
   <si>
@@ -1038,18 +1035,9 @@
     <t>Imm Injectiion</t>
   </si>
   <si>
-    <t>Type 1</t>
-  </si>
-  <si>
-    <t>Type 2</t>
-  </si>
-  <si>
     <t>Store</t>
   </si>
   <si>
-    <t>!must change which register it writes to memory</t>
-  </si>
-  <si>
     <t>regTSBeta</t>
   </si>
   <si>
@@ -1090,6 +1078,24 @@
   </si>
   <si>
     <t>RT</t>
+  </si>
+  <si>
+    <t>INSTRUCTION_SIZE</t>
+  </si>
+  <si>
+    <t>Instruction</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Need for load next instruction</t>
+  </si>
+  <si>
+    <t>Type 1 (track select = 0)</t>
+  </si>
+  <si>
+    <t>Type 2 (track select = 1)</t>
   </si>
 </sst>
 </file>
@@ -1646,8 +1652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
@@ -1782,36 +1788,8 @@
       <c r="A8" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B8" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="35"/>
-      <c r="J8" s="33" t="s">
-        <v>317</v>
-      </c>
-      <c r="K8" s="35"/>
-      <c r="L8" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="34"/>
-      <c r="P8" s="34"/>
-      <c r="Q8" s="34"/>
-      <c r="R8" s="34"/>
-      <c r="S8" s="34"/>
-      <c r="T8" s="34"/>
-      <c r="U8" s="35"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.5">
+    </row>
+    <row r="9" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -1824,11 +1802,11 @@
       <c r="F9" s="34"/>
       <c r="G9" s="35"/>
       <c r="H9" s="33" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I9" s="35"/>
       <c r="J9" s="33" t="s">
-        <v>14</v>
+        <v>313</v>
       </c>
       <c r="K9" s="35"/>
       <c r="L9" s="33" t="s">
@@ -1848,78 +1826,106 @@
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B10" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="35"/>
+      <c r="J10" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="35"/>
+      <c r="L10" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="34"/>
+      <c r="S10" s="34"/>
+      <c r="T10" s="34"/>
+      <c r="U10" s="35"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A11" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B11" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="35"/>
-      <c r="J11" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
-      <c r="P11" s="34"/>
-      <c r="Q11" s="34"/>
-      <c r="R11" s="34"/>
-      <c r="S11" s="34"/>
-      <c r="T11" s="34"/>
-      <c r="U11" s="35"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B12" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="35"/>
+      <c r="J12" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="34"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="34"/>
+      <c r="T12" s="34"/>
+      <c r="U12" s="35"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="34"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="R13" s="34"/>
-      <c r="S13" s="34"/>
-      <c r="T13" s="34"/>
-      <c r="U13" s="35"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="B14" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="R14" s="34"/>
+      <c r="S14" s="34"/>
+      <c r="T14" s="34"/>
+      <c r="U14" s="35"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A16" s="27"/>
@@ -1992,7 +1998,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A19" s="26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D19" s="31"/>
       <c r="E19" s="31"/>
@@ -2015,13 +2021,13 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A20" s="2" t="s">
-        <v>300</v>
+        <v>318</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D20" s="27"/>
       <c r="E20" s="27"/>
@@ -2047,7 +2053,7 @@
         <v>119</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C21" s="27">
         <v>1</v>
@@ -2076,7 +2082,7 @@
         <v>120</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C22" s="31">
         <v>2</v>
@@ -2102,7 +2108,7 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A23" s="27" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="27"/>
@@ -2127,7 +2133,7 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A24" s="27" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B24" s="31"/>
       <c r="C24" s="31"/>
@@ -2175,10 +2181,10 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A26" s="2" t="s">
-        <v>301</v>
+        <v>319</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C26" s="31">
         <v>1</v>
@@ -2207,7 +2213,7 @@
         <v>121</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C27" s="27">
         <v>2</v>
@@ -2233,16 +2239,14 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A28" s="27" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B28" s="31" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C28" s="31"/>
       <c r="D28" s="27"/>
-      <c r="E28" s="27" t="s">
-        <v>303</v>
-      </c>
+      <c r="E28" s="27"/>
       <c r="F28" s="27"/>
       <c r="G28" s="27"/>
       <c r="H28" s="27"/>
@@ -2316,20 +2320,20 @@
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:U8"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:U11"/>
-    <mergeCell ref="Q13:U13"/>
-    <mergeCell ref="H13:P13"/>
+    <mergeCell ref="B14:G14"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:U9"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J12:U12"/>
+    <mergeCell ref="Q14:U14"/>
+    <mergeCell ref="H14:P14"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:U10"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
@@ -2345,8 +2349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2897DEC3-240E-431E-8285-E03640E230E7}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.5" x14ac:dyDescent="0.45"/>
@@ -2486,7 +2490,7 @@
       <c r="F10" s="17"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A11" s="15"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
@@ -2737,8 +2741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E23297D-859B-4DF0-AD52-FCC5F95569EC}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
@@ -3138,15 +3142,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A9AC7C-0DA4-46BC-A427-30A253EEB689}">
   <dimension ref="A1:AK13"/>
   <sheetViews>
-    <sheetView topLeftCell="AF1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AK21" sqref="AK21"/>
+    <sheetView topLeftCell="U1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="41.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -3161,10 +3165,10 @@
     <col min="15" max="15" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="49.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="41.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="43.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="41.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="41.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="43" style="1" customWidth="1"/>
     <col min="24" max="24" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -3471,7 +3475,7 @@
         <v>106</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>102</v>
+        <v>315</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="1" t="s">
@@ -3485,7 +3489,7 @@
         <v>106</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>103</v>
+        <v>315</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="1" t="s">
@@ -3506,21 +3510,21 @@
         <v>106</v>
       </c>
       <c r="R4" s="10" t="s">
-        <v>103</v>
+        <v>315</v>
       </c>
       <c r="S4" s="12"/>
       <c r="T4" s="1" t="s">
         <v>106</v>
       </c>
       <c r="U4" s="10" t="s">
-        <v>103</v>
+        <v>315</v>
       </c>
       <c r="V4" s="12"/>
       <c r="W4" s="1" t="s">
         <v>106</v>
       </c>
       <c r="X4" s="10" t="s">
-        <v>103</v>
+        <v>316</v>
       </c>
       <c r="Y4" s="12"/>
       <c r="Z4" s="1" t="s">
@@ -3536,7 +3540,7 @@
         <v>106</v>
       </c>
       <c r="AD4" s="10" t="s">
-        <v>107</v>
+        <v>316</v>
       </c>
       <c r="AE4" s="12"/>
       <c r="AF4" s="1" t="s">
@@ -3623,7 +3627,7 @@
         <v>102</v>
       </c>
       <c r="Y5" s="12" t="s">
-        <v>113</v>
+        <v>317</v>
       </c>
       <c r="Z5" s="1" t="s">
         <v>84</v>
@@ -4431,8 +4435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EAB20A-8932-4835-BF8E-F6B57D7CCDEF}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A33" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
@@ -4446,16 +4450,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>247</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.5">
@@ -4463,13 +4467,13 @@
         <v>67</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C2" s="29">
         <v>1</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.5">
@@ -4477,13 +4481,13 @@
         <v>67</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.5">
@@ -4491,13 +4495,13 @@
         <v>67</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C4" s="29">
         <v>3</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.5">
@@ -4505,32 +4509,32 @@
         <v>67</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C5" s="30">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>251</v>
       </c>
       <c r="C6" s="30">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>166</v>
@@ -4539,105 +4543,105 @@
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="C8" s="30">
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C9" s="30">
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C10" s="30">
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C11" s="30">
         <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C12" s="30">
         <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C13" s="30">
         <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C14" s="30">
         <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.5">
@@ -4645,97 +4649,97 @@
         <v>166</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C15" s="30">
         <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C16" s="30">
         <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C17" s="30">
         <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C18" s="30">
         <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C19" s="30">
         <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C20" s="30">
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C21" s="30">
         <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.5">
@@ -4743,46 +4747,46 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C22" s="30">
         <v>21</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C23" s="30">
         <v>22</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C24" s="30">
         <v>23</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>149</v>
@@ -4791,49 +4795,49 @@
         <v>24</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C26" s="30">
         <v>25</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A27" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C27" s="30">
         <v>26</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C28" s="30">
         <v>27</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.5">
@@ -4841,13 +4845,13 @@
         <v>149</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C29" s="30">
         <v>28</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.5">
@@ -4855,13 +4859,13 @@
         <v>149</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C30" s="30">
         <v>29</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.5">
@@ -4869,32 +4873,32 @@
         <v>149</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C31" s="30">
         <v>30</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A32" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C32" s="30">
         <v>31</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A33" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>67</v>
@@ -4903,194 +4907,194 @@
         <v>32</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A34" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C34" s="30">
         <v>33</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A35" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C35" s="30">
         <v>34</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A36" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C36" s="30">
         <v>35</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A37" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C37" s="30">
         <v>36</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A38" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="C38" s="30">
         <v>37</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A39" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C39" s="30">
         <v>38</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A40" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C40" s="30">
         <v>39</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A41" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>274</v>
       </c>
       <c r="C41" s="30">
         <v>40</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A42" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C42" s="30">
         <v>41</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A43" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C43" s="30">
         <v>42</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A44" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C44" s="30">
         <v>43</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A45" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C45" s="30">
         <v>44</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A46" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C46" s="30">
         <v>45</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A47" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>67</v>
@@ -5099,63 +5103,63 @@
         <v>46</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A48" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C48" s="30">
         <v>47</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A49" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C49" s="30">
         <v>48</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A50" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>311</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>315</v>
       </c>
       <c r="C50" s="30">
         <v>49</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A51" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C51" s="30">
         <v>50</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -5170,10 +5174,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD505EFA-7D11-43A5-AB74-E1417C081A89}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
@@ -5244,7 +5248,7 @@
         <v>149</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.5">
@@ -5379,11 +5383,6 @@
       </c>
       <c r="B13" s="21" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B19" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Phase 1 Upload 1
</commit_message>
<xml_diff>
--- a/materials/Instructions.xlsx
+++ b/materials/Instructions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingi\Documents\UTD\4310 Arch\Project\materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756DDD9C-7841-4BE6-A7B8-CFA2D2E8CB36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3149891D-571B-4197-A477-020AD3134EB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="797" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="797" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction Types" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="318">
   <si>
     <t>Opcode</t>
   </si>
@@ -210,45 +210,9 @@
     <t>jump relative_address</t>
   </si>
   <si>
-    <t>mov R1 0</t>
-  </si>
-  <si>
-    <t>mov R2 0</t>
-  </si>
-  <si>
-    <t>start</t>
-  </si>
-  <si>
-    <t>done</t>
-  </si>
-  <si>
-    <t>mov R3 10</t>
-  </si>
-  <si>
-    <t>For i&lt;=10</t>
-  </si>
-  <si>
-    <t>R2 has i</t>
-  </si>
-  <si>
-    <t>R1 is sum</t>
-  </si>
-  <si>
-    <t>b R2 &gt; R3 : done</t>
-  </si>
-  <si>
     <t>loop</t>
   </si>
   <si>
-    <t>add R1 R1 R2</t>
-  </si>
-  <si>
-    <t>j loop</t>
-  </si>
-  <si>
-    <t>add R2 R2 1</t>
-  </si>
-  <si>
     <t>add RD R1 imm</t>
   </si>
   <si>
@@ -567,9 +531,6 @@
     <t>ALU R (Step 3)</t>
   </si>
   <si>
-    <t>Imm Injection (Step 2)</t>
-  </si>
-  <si>
     <t>need for next instruction</t>
   </si>
   <si>
@@ -672,9 +633,6 @@
     <t>000</t>
   </si>
   <si>
-    <t>001</t>
-  </si>
-  <si>
     <t>010</t>
   </si>
   <si>
@@ -1096,6 +1054,42 @@
   </si>
   <si>
     <t>Type 2 (track select = 1)</t>
+  </si>
+  <si>
+    <t>Imm Injection (Step 3)</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>R0</t>
+  </si>
+  <si>
+    <t>bgt</t>
+  </si>
+  <si>
+    <t>.finish</t>
+  </si>
+  <si>
+    <t>addi</t>
+  </si>
+  <si>
+    <t>.loop</t>
+  </si>
+  <si>
+    <t>Execution Breakdown</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">load </t>
+  </si>
+  <si>
+    <t>Total Clocks</t>
+  </si>
+  <si>
+    <t>CPI</t>
   </si>
 </sst>
 </file>
@@ -1304,7 +1298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1368,6 +1362,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1653,7 +1650,7 @@
   <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="B3" sqref="B3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
@@ -1665,7 +1662,7 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="B1" s="32" t="s">
         <v>0</v>
@@ -1688,7 +1685,7 @@
       </c>
       <c r="M1" s="32"/>
       <c r="N1" s="33" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="O1" s="34"/>
       <c r="P1" s="34"/>
@@ -1705,7 +1702,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B3" s="32" t="s">
         <v>0</v>
@@ -1738,7 +1735,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.5">
@@ -1781,12 +1778,12 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A8" s="2" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
@@ -1806,7 +1803,7 @@
       </c>
       <c r="I9" s="35"/>
       <c r="J9" s="33" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="K9" s="35"/>
       <c r="L9" s="33" t="s">
@@ -1857,7 +1854,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A11" s="2" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.5">
@@ -1909,7 +1906,7 @@
       <c r="F14" s="34"/>
       <c r="G14" s="35"/>
       <c r="H14" s="33" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="I14" s="34"/>
       <c r="J14" s="34"/>
@@ -1920,7 +1917,7 @@
       <c r="O14" s="34"/>
       <c r="P14" s="35"/>
       <c r="Q14" s="33" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="R14" s="34"/>
       <c r="S14" s="34"/>
@@ -1998,7 +1995,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A19" s="26" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="D19" s="31"/>
       <c r="E19" s="31"/>
@@ -2021,13 +2018,13 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A20" s="2" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="D20" s="27"/>
       <c r="E20" s="27"/>
@@ -2050,10 +2047,10 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A21" s="27" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="C21" s="27">
         <v>1</v>
@@ -2079,10 +2076,10 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A22" s="27" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="C22" s="31">
         <v>2</v>
@@ -2108,7 +2105,7 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A23" s="27" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="27"/>
@@ -2133,7 +2130,7 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A24" s="27" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="B24" s="31"/>
       <c r="C24" s="31"/>
@@ -2181,10 +2178,10 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A26" s="2" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="C26" s="31">
         <v>1</v>
@@ -2210,10 +2207,10 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A27" s="27" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="C27" s="27">
         <v>2</v>
@@ -2239,10 +2236,10 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A28" s="27" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="B28" s="31" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="C28" s="31"/>
       <c r="D28" s="27"/>
@@ -2312,14 +2309,11 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:U3"/>
-    <mergeCell ref="L5:U5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:U1"/>
     <mergeCell ref="B14:G14"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="H9:I9"/>
@@ -2334,11 +2328,14 @@
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="L10:U10"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:U3"/>
+    <mergeCell ref="L5:U5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2349,8 +2346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2897DEC3-240E-431E-8285-E03640E230E7}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G2"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.5" x14ac:dyDescent="0.45"/>
@@ -2367,33 +2364,33 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
@@ -2403,64 +2400,64 @@
     </row>
     <row r="3" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="36" t="s">
-        <v>123</v>
-      </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="6" t="s">
-        <v>130</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
     </row>
     <row r="4" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="G4" s="18"/>
+        <v>114</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C5" s="38"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F5" s="18"/>
       <c r="G5" s="18"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="18"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
@@ -2481,7 +2478,7 @@
     </row>
     <row r="10" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="17" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
@@ -2538,27 +2535,27 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" s="5" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47" s="5" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B47" s="36" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C47" s="36"/>
       <c r="D47" s="36"/>
@@ -2566,10 +2563,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" s="5" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B48" s="36" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C48" s="36"/>
       <c r="D48" s="36"/>
@@ -2577,65 +2574,65 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B49" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="D49" s="6" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="57" x14ac:dyDescent="0.45">
       <c r="A50" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B50" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B50" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="C50" s="6" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" s="5" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B51" s="6"/>
       <c r="C51" s="6" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B53" s="5" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" s="5" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B54" s="36" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C54" s="36"/>
       <c r="D54" s="36"/>
@@ -2643,10 +2640,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" s="5" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B55" s="36" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C55" s="36"/>
       <c r="D55" s="36"/>
@@ -2654,71 +2651,71 @@
     </row>
     <row r="56" spans="1:5" ht="57" x14ac:dyDescent="0.45">
       <c r="A56" s="5" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="57" x14ac:dyDescent="0.45">
       <c r="A57" s="5" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" s="5" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B58" s="6"/>
       <c r="C58" s="6" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61" s="4" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B62" s="4" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B63" s="4" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B64" s="4" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B65" s="4" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2728,8 +2725,8 @@
     <mergeCell ref="B54:E54"/>
     <mergeCell ref="B55:E55"/>
     <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:F3"/>
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2742,7 +2739,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
@@ -2762,79 +2759,79 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.5">
       <c r="B1" s="1" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="F1" s="27"/>
       <c r="G1" s="15" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="H1" s="15"/>
       <c r="I1" s="27"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A2" s="19" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="H2" s="28" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="I2" s="27"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A3" s="19" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="I3" s="27"/>
       <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A4" s="19" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="I4" s="28"/>
       <c r="J4" s="25"/>
@@ -2842,22 +2839,22 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A5" s="19" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="H5" s="28" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="I5" s="28"/>
       <c r="J5" s="25"/>
@@ -2865,22 +2862,22 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A6" s="19" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="I6" s="28"/>
       <c r="J6" s="25"/>
@@ -2888,22 +2885,22 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A7" s="19" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>182</v>
+        <v>307</v>
       </c>
       <c r="I7" s="28"/>
       <c r="J7" s="25"/>
@@ -2911,13 +2908,13 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.5">
       <c r="E8" s="28" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="H8" s="28"/>
       <c r="I8" s="28"/>
@@ -2926,16 +2923,16 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.5">
       <c r="E9" s="28" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="I9" s="28"/>
       <c r="J9" s="25"/>
@@ -2943,16 +2940,16 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.5">
       <c r="E10" s="28" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="I10" s="28"/>
       <c r="J10" s="25"/>
@@ -2960,13 +2957,13 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.5">
       <c r="E11" s="28" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="H11" s="28"/>
       <c r="I11" s="28"/>
@@ -2975,16 +2972,16 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.5">
       <c r="E12" s="28" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="H12" s="28" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="I12" s="28"/>
       <c r="J12" s="25"/>
@@ -2992,25 +2989,25 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A13" s="2" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="E13" s="27"/>
       <c r="F13" s="27"/>
       <c r="G13" s="26" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H13" s="28"/>
       <c r="I13" s="27"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="G14" s="25" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="H14" s="25">
         <v>111111</v>
@@ -3018,118 +3015,118 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G15" s="25"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A27" s="1" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A32" s="1" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A33" s="1" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A34" s="1" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A35" s="1" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A36" s="1" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A37" s="1" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -3142,8 +3139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A9AC7C-0DA4-46BC-A427-30A253EEB689}">
   <dimension ref="A1:AK13"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
@@ -3187,1243 +3184,1243 @@
   <sheetData>
     <row r="1" spans="1:37" s="8" customFormat="1" ht="114" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>143</v>
+        <v>306</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="K1" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="R1" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="S1" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="T1" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="U1" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="V1" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="W1" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="L1" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q1" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="R1" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="S1" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="T1" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="U1" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="V1" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="W1" s="13" t="s">
-        <v>155</v>
-      </c>
       <c r="X1" s="14" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="Y1" s="11" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="Z1" s="13" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="AA1" s="14" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="AB1" s="11" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="AC1" s="13" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="AD1" s="14" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="AE1" s="11" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="AF1" s="13" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="AG1" s="14" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="AH1" s="11" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="AI1" s="13" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="AJ1" s="14" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="AK1" s="11" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:37" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C2" s="10">
         <v>1</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="M2" s="12"/>
       <c r="N2" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="P2" s="12"/>
       <c r="Q2" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="R2" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="S2" s="12"/>
       <c r="T2" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="U2" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="V2" s="12"/>
       <c r="W2" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="X2" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Y2" s="12"/>
       <c r="Z2" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="AA2" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AB2" s="12"/>
       <c r="AC2" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="AD2" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AE2" s="12"/>
       <c r="AF2" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="AG2" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AH2" s="12"/>
       <c r="AI2" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="AJ2" s="10" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="AK2" s="12"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.5">
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="J3" s="12"/>
       <c r="K3" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="M3" s="12"/>
       <c r="N3" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="P3" s="12"/>
       <c r="Q3" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="R3" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="S3" s="12"/>
       <c r="T3" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="U3" s="10" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="V3" s="12"/>
       <c r="W3" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="X3" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Y3" s="12"/>
       <c r="Z3" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="AA3" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AB3" s="12"/>
       <c r="AC3" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="AD3" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AE3" s="12"/>
       <c r="AF3" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="AG3" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AH3" s="12"/>
       <c r="AI3" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="AJ3" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AK3" s="12"/>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.5">
       <c r="B4" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="M4" s="12"/>
       <c r="N4" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="P4" s="12"/>
       <c r="Q4" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="R4" s="10" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="S4" s="12"/>
       <c r="T4" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="U4" s="10" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="V4" s="12"/>
       <c r="W4" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="X4" s="10" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="Y4" s="12"/>
       <c r="Z4" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="AA4" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AB4" s="12" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="AD4" s="10" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="AE4" s="12"/>
       <c r="AF4" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="AG4" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AH4" s="12"/>
       <c r="AI4" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="AJ4" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AK4" s="12"/>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.5">
       <c r="B5" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="O5" s="10" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="R5" s="10" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="U5" s="10" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="V5" s="12" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="X5" s="10" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="Y5" s="12" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="AA5" s="10" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="AB5" s="12" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="AD5" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AE5" s="12" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="AF5" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="AG5" s="10" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="AH5" s="12" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="AI5" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="AJ5" s="10" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="AK5" s="12" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.5">
       <c r="B6" s="1" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="1" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="M6" s="12"/>
       <c r="N6" s="1" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="O6" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="P6" s="12"/>
       <c r="Q6" s="1" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="R6" s="10" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="S6" s="12"/>
       <c r="T6" s="1" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="U6" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="V6" s="12"/>
       <c r="W6" s="1" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="X6" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="Y6" s="12"/>
       <c r="Z6" s="1" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="AA6" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AB6" s="12"/>
       <c r="AC6" s="1" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="AD6" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AE6" s="12"/>
       <c r="AF6" s="1" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="AG6" s="10" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="AH6" s="12"/>
       <c r="AI6" s="1" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="AJ6" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AK6" s="12"/>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.5">
       <c r="B7" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="P7" s="12" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="R7" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="S7" s="12" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="U7" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="V7" s="12" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="X7" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Y7" s="12" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="AA7" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AB7" s="12" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="AD7" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AE7" s="12" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="AF7" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="AG7" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AH7" s="12" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="AI7" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="AJ7" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AK7" s="12" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:37" hidden="1" x14ac:dyDescent="0.5">
       <c r="B8" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="O8" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="P8" s="12"/>
       <c r="Q8" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="R8" s="10" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="S8" s="12"/>
       <c r="T8" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="U8" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="V8" s="12"/>
       <c r="W8" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="X8" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="Y8" s="12" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="AA8" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AB8" s="12" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="AD8" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AE8" s="12" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="AF8" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="AG8" s="10" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="AH8" s="12" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="AI8" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="AJ8" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AK8" s="12" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.5">
       <c r="B9" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="O9" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="P9" s="12"/>
       <c r="Q9" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="R9" s="10" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="S9" s="12"/>
       <c r="T9" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="U9" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="V9" s="12"/>
       <c r="W9" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="X9" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="Y9" s="12"/>
       <c r="Z9" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="AA9" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AB9" s="12"/>
       <c r="AC9" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="AD9" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AE9" s="12"/>
       <c r="AF9" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="AG9" s="10" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="AH9" s="12"/>
       <c r="AI9" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="AJ9" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="AK9" s="12"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.5">
       <c r="B10" s="1" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="1" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="1" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="M10" s="12"/>
       <c r="N10" s="1" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="O10" s="10" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="P10" s="12"/>
       <c r="Q10" s="1" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="R10" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="S10" s="12"/>
       <c r="T10" s="1" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="U10" s="10" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="V10" s="12"/>
       <c r="W10" s="1" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="X10" s="10" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="Y10" s="12"/>
       <c r="Z10" s="1" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="AA10" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AB10" s="12"/>
       <c r="AC10" s="1" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="AD10" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AE10" s="12"/>
       <c r="AF10" s="1" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="AG10" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AH10" s="12"/>
       <c r="AI10" s="1" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="AJ10" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AK10" s="12"/>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.5">
       <c r="B11" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="M11" s="12"/>
       <c r="N11" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="O11" s="10" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="P11" s="12"/>
       <c r="Q11" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="R11" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="S11" s="12"/>
       <c r="T11" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="U11" s="10" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="V11" s="12"/>
       <c r="W11" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="X11" s="10" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="Y11" s="12"/>
       <c r="Z11" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="AA11" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AB11" s="12"/>
       <c r="AC11" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="AD11" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AE11" s="12"/>
       <c r="AF11" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="AG11" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AH11" s="12"/>
       <c r="AI11" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="AJ11" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AK11" s="12"/>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.5">
       <c r="B12" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="M12" s="12"/>
       <c r="N12" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="O12" s="10" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="P12" s="12"/>
       <c r="Q12" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="R12" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="S12" s="12"/>
       <c r="T12" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="U12" s="10" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="V12" s="12"/>
       <c r="W12" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="X12" s="10" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="Y12" s="12"/>
       <c r="Z12" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="AA12" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AB12" s="12"/>
       <c r="AC12" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="AD12" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AE12" s="12"/>
       <c r="AF12" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="AG12" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AH12" s="12"/>
       <c r="AI12" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="AJ12" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AK12" s="12"/>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.5">
       <c r="B13" s="1" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="1" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="I13" s="10">
         <v>0</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="O13" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="P13" s="12" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="R13" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="S13" s="12" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="U13" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="V13" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="X13" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y13" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA13" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB13" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AD13" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE13" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="AF13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG13" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH13" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="AI13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ13" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="V13" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="W13" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="X13" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="Y13" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="Z13" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AA13" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB13" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="AC13" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AD13" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="AE13" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="AF13" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AG13" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="AH13" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="AI13" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AJ13" s="10" t="s">
-        <v>167</v>
-      </c>
       <c r="AK13" s="12" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -4435,8 +4432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EAB20A-8932-4835-BF8E-F6B57D7CCDEF}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView topLeftCell="A17" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
@@ -4450,296 +4447,296 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" s="29" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="C2" s="29">
         <v>1</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A4" s="29" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="C4" s="29">
         <v>3</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="C5" s="30">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="C6" s="30">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="C7" s="30">
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="C8" s="30">
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="C9" s="30">
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="C10" s="30">
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="C11" s="30">
         <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="C12" s="30">
         <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>264</v>
       </c>
       <c r="C13" s="30">
         <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="C14" s="30">
         <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="C15" s="30">
         <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="C16" s="30">
         <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="C17" s="30">
         <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="C18" s="30">
         <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="C19" s="30">
         <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="C20" s="30">
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="C21" s="30">
         <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.5">
@@ -4747,419 +4744,419 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="C22" s="30">
         <v>21</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="C23" s="30">
         <v>22</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="C24" s="30">
         <v>23</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="C25" s="30">
         <v>24</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="C26" s="30">
         <v>25</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A27" s="1" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="C27" s="30">
         <v>26</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="C28" s="30">
         <v>27</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="C29" s="30">
         <v>28</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="C30" s="30">
         <v>29</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="C31" s="30">
         <v>30</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A32" s="1" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="C32" s="30">
         <v>31</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A33" s="1" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C33" s="30">
         <v>32</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A34" s="1" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="C34" s="30">
         <v>33</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A35" s="1" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="C35" s="30">
         <v>34</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A36" s="1" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="C36" s="30">
         <v>35</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A37" s="1" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="C37" s="30">
         <v>36</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A38" s="1" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="C38" s="30">
         <v>37</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A39" s="1" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="C39" s="30">
         <v>38</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A40" s="1" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="C40" s="30">
         <v>39</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A41" s="1" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="C41" s="30">
         <v>40</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A42" s="1" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="C42" s="30">
         <v>41</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A43" s="1" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="C43" s="30">
         <v>42</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A44" s="1" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="C44" s="30">
         <v>43</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A45" s="1" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="C45" s="30">
         <v>44</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A46" s="1" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="C46" s="30">
         <v>45</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A47" s="1" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C47" s="30">
         <v>46</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A48" s="1" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="C48" s="30">
         <v>47</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A49" s="1" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="C49" s="30">
         <v>48</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A50" s="1" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="C50" s="30">
         <v>49</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A51" s="1" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
       <c r="C51" s="30">
         <v>50</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -5196,107 +5193,107 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A1" s="20" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" s="21" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="E2" s="22">
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A3" s="21" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="E3" s="22">
         <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A4" s="24" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="E4" s="22">
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5" s="21" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="E5" s="22">
         <v>2</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6" s="24" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="E6" s="22">
         <v>4</v>
@@ -5305,84 +5302,84 @@
         <v>4</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A7" s="21" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E7" s="22">
         <v>4</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A8" s="23" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A9" s="21" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A10" s="24" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A11" s="24" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A12" s="21" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A13" s="24" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -5393,87 +5390,221 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB8343A-D685-4ED2-8392-538E9DE143BE}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="33.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="9.140625" style="3"/>
+    <col min="9" max="9" width="46.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
-        <v>26</v>
-      </c>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
       <c r="B1" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="D1" s="3">
+        <v>0</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="B2" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="B3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3">
+        <v>10</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="J3" s="3">
+        <v>3</v>
+      </c>
+      <c r="K3" s="3">
+        <v>3</v>
+      </c>
+      <c r="L3" s="3">
+        <f>K3*J3</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="J4" s="3">
+        <v>12</v>
+      </c>
+      <c r="K4" s="3">
+        <v>3</v>
+      </c>
+      <c r="L4" s="3">
+        <f t="shared" ref="L4:L8" si="0">K4*J4</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="B5" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="J5" s="3">
+        <v>11</v>
+      </c>
+      <c r="K5" s="3">
+        <v>4</v>
+      </c>
+      <c r="L5" s="3">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="B6" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="J6" s="3">
+        <v>11</v>
+      </c>
+      <c r="K6" s="3">
+        <v>4</v>
+      </c>
+      <c r="L6" s="3">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="B7" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J7" s="3">
+        <v>11</v>
+      </c>
+      <c r="K7" s="3">
+        <v>3</v>
+      </c>
+      <c r="L7" s="3">
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" ht="33.75" x14ac:dyDescent="0.5">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+        <v>310</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="J8" s="3">
+        <v>1</v>
+      </c>
+      <c r="K8" s="3">
+        <v>4</v>
+      </c>
+      <c r="L8" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="L9" s="3">
+        <f>SUM(L3:L8)</f>
+        <v>170</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5574,7 +5705,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B1" s="7">
         <v>0</v>
@@ -5637,7 +5768,7 @@
         <v>19</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.5">
@@ -5662,7 +5793,7 @@
       </c>
       <c r="M2" s="35"/>
       <c r="N2" s="33" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="O2" s="34"/>
       <c r="P2" s="34"/>
@@ -5672,7 +5803,7 @@
       <c r="T2" s="34"/>
       <c r="U2" s="35"/>
       <c r="V2" s="1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.5">
@@ -5705,7 +5836,7 @@
       <c r="T3" s="34"/>
       <c r="U3" s="35"/>
       <c r="V3" s="1" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.5">
@@ -5806,7 +5937,7 @@
       <c r="F7" s="34"/>
       <c r="G7" s="35"/>
       <c r="H7" s="33" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="I7" s="34"/>
       <c r="J7" s="34"/>
@@ -5819,13 +5950,26 @@
       <c r="Q7" s="34"/>
       <c r="R7" s="35"/>
       <c r="S7" s="33" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="T7" s="34"/>
       <c r="U7" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:U2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:U3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:U4"/>
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="H7:R7"/>
     <mergeCell ref="S7:U7"/>
@@ -5836,19 +5980,6 @@
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="J6:U6"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:U3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:U4"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:U2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Submit for Revised Phase 1 Instructions
</commit_message>
<xml_diff>
--- a/materials/Instructions.xlsx
+++ b/materials/Instructions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingi\Documents\UTD\4310 Arch\Project\materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3149891D-571B-4197-A477-020AD3134EB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F18AF20-3DDA-4BEF-A3B4-90CD74AD251D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="797" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="797" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction Types" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="326">
   <si>
     <t>Opcode</t>
   </si>
@@ -1090,6 +1090,30 @@
   </si>
   <si>
     <t>CPI</t>
+  </si>
+  <si>
+    <t>BEQ</t>
+  </si>
+  <si>
+    <t>BNEQ</t>
+  </si>
+  <si>
+    <t>BLT</t>
+  </si>
+  <si>
+    <t>BLEQ</t>
+  </si>
+  <si>
+    <t>BGT</t>
+  </si>
+  <si>
+    <t>BGEQ</t>
+  </si>
+  <si>
+    <t>STR</t>
+  </si>
+  <si>
+    <t>JUMP</t>
   </si>
 </sst>
 </file>
@@ -1649,8 +1673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:G3"/>
+    <sheetView topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11:W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
@@ -2347,7 +2371,7 @@
   <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.5" x14ac:dyDescent="0.45"/>
@@ -2736,10 +2760,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E23297D-859B-4DF0-AD52-FCC5F95569EC}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
@@ -3001,102 +3025,107 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="G14" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="H14" s="25">
-        <v>111111</v>
-      </c>
+        <v>325</v>
+      </c>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="27"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="G15" s="25"/>
+        <v>204</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="H15" s="25">
+        <v>111111</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
-        <v>207</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="G16" s="25"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A27" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.5">
@@ -3106,27 +3135,72 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A33" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A34" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A35" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A36" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A37" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A38" s="1" t="s">
         <v>227</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A39" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A40" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A41" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A42" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A43" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A44" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A45" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A46" s="1" t="s">
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -5392,8 +5466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB8343A-D685-4ED2-8392-538E9DE143BE}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="33.75" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
Changed the the parameters that were used in opcodes.v and ControlStates.v to "Verilog Headers" that use the preprocessor defines
</commit_message>
<xml_diff>
--- a/materials/Instructions.xlsx
+++ b/materials/Instructions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingi\Documents\UTD\4310 Arch\Project\materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingi\Documents\UTD\4310-Arch\Project\materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756DDD9C-7841-4BE6-A7B8-CFA2D2E8CB36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F036924-8B84-4136-B014-3BB8A751BE5C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="797" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2312,14 +2312,11 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:U3"/>
-    <mergeCell ref="L5:U5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:U1"/>
     <mergeCell ref="B14:G14"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="H9:I9"/>
@@ -2334,11 +2331,14 @@
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="L10:U10"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:U3"/>
+    <mergeCell ref="L5:U5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2349,8 +2349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2897DEC3-240E-431E-8285-E03640E230E7}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.5" x14ac:dyDescent="0.45"/>
@@ -5826,6 +5826,19 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:U2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:U3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:U4"/>
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="H7:R7"/>
     <mergeCell ref="S7:U7"/>
@@ -5836,19 +5849,6 @@
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="J6:U6"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:U3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:U4"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:U2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>